<commit_message>
fixed: image and description is fixed
</commit_message>
<xml_diff>
--- a/Data/amorethica_products.xlsx
+++ b/Data/amorethica_products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,6 +539,11 @@
           <t>Variant Inventory Qty</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -563,18 +568,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>&lt;div class="wd-negative-gap elementor-element elementor-element-aa67a64 wd-section-stretch wd-collapsible-content e-flex e-con-boxed e-con e-parent" data-element_type="container" data-id="aa67a64"&gt;
-&lt;div class="e-con-inner"&gt;
-&lt;div class="elementor-element elementor-element-81ef30d wd-width-100 elementor-widget elementor-widget-wd_title" data-element_type="widget" data-id="81ef30d" data-widget_type="wd_title.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-section-title.min.css?ver=8.1.1" id="wd-section-title-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="title-wrapper wd-set-mb reset-last-child wd-title-color-default wd-title-style-default wd-title-size-default text-left"&gt;
-&lt;div class="liner-continer"&gt;
-&lt;h4 class="woodmart-title-container title wd-fontsize-l"&gt;Features &amp;amp; Compatibility&lt;/h4&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
+          <t>&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
 &lt;div class="elementor-widget-container"&gt;
 &lt;p&gt;Inspired by the moon’s mystique, the Luna Ring captures the night’s romance with its luminous diamond centerpiece.&lt;/p&gt;
 &lt;ul&gt;
@@ -586,20 +580,6 @@
 &lt;li&gt;Perfect for every woman&lt;/li&gt;
 &lt;/ul&gt;
 &lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-c127cd8 elementor-widget elementor-widget-wd_button" data-element_type="widget" data-id="c127cd8" data-widget_type="wd_button.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-button.min.css?ver=8.1.1" id="wd-button-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="wd-button-wrapper text-center wd-collapsible-button"&gt;
-&lt;a class="btn btn-style-link btn-shape- btn-size-default btn-color-primary btn-icon-pos-right" href="#"&gt;
-&lt;span class="wd-btn-text" data-elementor-setting-key="text"&gt;
-					SHOW MORE				&lt;/span&gt;
-&lt;span class="wd-btn-icon"&gt;
-&lt;svg class="wd-icon e-font-icon-svg e-fas-chevron-down" viewbox="0 0 448 512" xmlns="http://www.w3.org/2000/svg"&gt;&lt;path d="M207.029 381.476L12.686 187.132c-9.373-9.373-9.373-24.569 0-33.941l22.667-22.667c9.357-9.357 24.522-9.375 33.901-.04L224 284.505l154.745-154.021c9.379-9.335 24.544-9.317 33.901.04l22.667 22.667c9.373 9.373 9.373 24.569 0 33.941L240.971 381.476c-9.373 9.372-24.569 9.372-33.942 0z"&gt;&lt;/path&gt;&lt;/svg&gt; &lt;/span&gt;
-&lt;/a&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
 &lt;/div&gt;</t>
         </is>
       </c>
@@ -651,7 +631,12 @@
       </c>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>men</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -677,18 +662,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>&lt;div class="wd-negative-gap elementor-element elementor-element-aa67a64 wd-section-stretch wd-collapsible-content e-flex e-con-boxed e-con e-parent" data-element_type="container" data-id="aa67a64"&gt;
-&lt;div class="e-con-inner"&gt;
-&lt;div class="elementor-element elementor-element-81ef30d wd-width-100 elementor-widget elementor-widget-wd_title" data-element_type="widget" data-id="81ef30d" data-widget_type="wd_title.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-section-title.min.css?ver=8.1.1" id="wd-section-title-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="title-wrapper wd-set-mb reset-last-child wd-title-color-default wd-title-style-default wd-title-size-default text-left"&gt;
-&lt;div class="liner-continer"&gt;
-&lt;h4 class="woodmart-title-container title wd-fontsize-l"&gt;Features &amp;amp; Compatibility&lt;/h4&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
+          <t>&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
 &lt;div class="elementor-widget-container"&gt;
 &lt;p&gt;The Elara Ring, with its pavé diamond arrangement, promises eternal brilliance and grace. Featuring Emerald diamond it’s a classic twist of a perfect engagement ring.&lt;/p&gt;
 &lt;p&gt;￼&lt;/p&gt;
@@ -705,21 +679,7 @@
 &lt;li&gt;Perfect for every woman&lt;/li&gt;
 &lt;/ul&gt;
 &lt;p&gt;This piece is Custom made to order. Expected delivery within 7-10 days. Upon completion, your new heirloom will be dispatched using your chosen shipping method selected at checkout.&lt;/p&gt;
-&lt;p&gt;Have a special date in mind? Reach out to &lt;a class="__cf_email__" data-cfemail="97e4f6fbf2e4d7f6faf8e5f2e3fffef4f6b9f4f8fa" href="/cdn-cgi/l/email-protection"&gt;[email protected]&lt;/a&gt; as we may be able to accommodate a rush order for you.&lt;/p&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-c127cd8 elementor-widget elementor-widget-wd_button" data-element_type="widget" data-id="c127cd8" data-widget_type="wd_button.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-button.min.css?ver=8.1.1" id="wd-button-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="wd-button-wrapper text-center wd-collapsible-button"&gt;
-&lt;a class="btn btn-style-link btn-shape- btn-size-default btn-color-primary btn-icon-pos-right" href="#"&gt;
-&lt;span class="wd-btn-text" data-elementor-setting-key="text"&gt;
-					SHOW MORE				&lt;/span&gt;
-&lt;span class="wd-btn-icon"&gt;
-&lt;svg class="wd-icon e-font-icon-svg e-fas-chevron-down" viewbox="0 0 448 512" xmlns="http://www.w3.org/2000/svg"&gt;&lt;path d="M207.029 381.476L12.686 187.132c-9.373-9.373-9.373-24.569 0-33.941l22.667-22.667c9.357-9.357 24.522-9.375 33.901-.04L224 284.505l154.745-154.021c9.379-9.335 24.544-9.317 33.901.04l22.667 22.667c9.373 9.373 9.373 24.569 0 33.941L240.971 381.476c-9.373 9.372-24.569 9.372-33.942 0z"&gt;&lt;/path&gt;&lt;/svg&gt; &lt;/span&gt;
-&lt;/a&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
+&lt;p&gt;Have a special date in mind? Reach out to &lt;a class="__cf_email__" data-cfemail="f380929f9680b3929e9c8196879b9a9092dd909c9e" href="/cdn-cgi/l/email-protection"&gt;[email protected]&lt;/a&gt; as we may be able to accommodate a rush order for you.&lt;/p&gt;
 &lt;/div&gt;
 &lt;/div&gt;</t>
         </is>
@@ -772,7 +732,12 @@
       </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>men</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -798,18 +763,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>&lt;div class="wd-negative-gap elementor-element elementor-element-aa67a64 wd-section-stretch wd-collapsible-content e-flex e-con-boxed e-con e-parent" data-element_type="container" data-id="aa67a64"&gt;
-&lt;div class="e-con-inner"&gt;
-&lt;div class="elementor-element elementor-element-81ef30d wd-width-100 elementor-widget elementor-widget-wd_title" data-element_type="widget" data-id="81ef30d" data-widget_type="wd_title.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-section-title.min.css?ver=8.1.1" id="wd-section-title-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="title-wrapper wd-set-mb reset-last-child wd-title-color-default wd-title-style-default wd-title-size-default text-left"&gt;
-&lt;div class="liner-continer"&gt;
-&lt;h4 class="woodmart-title-container title wd-fontsize-l"&gt;Features &amp;amp; Compatibility&lt;/h4&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
+          <t>&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
 &lt;div class="elementor-widget-container"&gt;
 &lt;p&gt;Our Tennis Bracelet wraps your wrist in a shimmer of stars, dazzling with every flicker. Called after a tennis star Chris Evert, when she stopped the match to find her beloved diamond bracelet in 1978.&lt;/p&gt;
 &lt;ul&gt;
@@ -823,20 +777,6 @@
 &lt;li&gt;Classic 4 prong setting&lt;/li&gt;
 &lt;/ul&gt;
 &lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-c127cd8 elementor-widget elementor-widget-wd_button" data-element_type="widget" data-id="c127cd8" data-widget_type="wd_button.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-button.min.css?ver=8.1.1" id="wd-button-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="wd-button-wrapper text-center wd-collapsible-button"&gt;
-&lt;a class="btn btn-style-link btn-shape- btn-size-default btn-color-primary btn-icon-pos-right" href="#"&gt;
-&lt;span class="wd-btn-text" data-elementor-setting-key="text"&gt;
-					SHOW MORE				&lt;/span&gt;
-&lt;span class="wd-btn-icon"&gt;
-&lt;svg class="wd-icon e-font-icon-svg e-fas-chevron-down" viewbox="0 0 448 512" xmlns="http://www.w3.org/2000/svg"&gt;&lt;path d="M207.029 381.476L12.686 187.132c-9.373-9.373-9.373-24.569 0-33.941l22.667-22.667c9.357-9.357 24.522-9.375 33.901-.04L224 284.505l154.745-154.021c9.379-9.335 24.544-9.317 33.901.04l22.667 22.667c9.373 9.373 9.373 24.569 0 33.941L240.971 381.476c-9.373 9.372-24.569 9.372-33.942 0z"&gt;&lt;/path&gt;&lt;/svg&gt; &lt;/span&gt;
-&lt;/a&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
 &lt;/div&gt;</t>
         </is>
       </c>
@@ -888,7 +828,12 @@
       </c>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>men</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -914,18 +859,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>&lt;div class="wd-negative-gap elementor-element elementor-element-aa67a64 wd-section-stretch wd-collapsible-content e-flex e-con-boxed e-con e-parent" data-element_type="container" data-id="aa67a64"&gt;
-&lt;div class="e-con-inner"&gt;
-&lt;div class="elementor-element elementor-element-81ef30d wd-width-100 elementor-widget elementor-widget-wd_title" data-element_type="widget" data-id="81ef30d" data-widget_type="wd_title.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-section-title.min.css?ver=8.1.1" id="wd-section-title-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="title-wrapper wd-set-mb reset-last-child wd-title-color-default wd-title-style-default wd-title-size-default text-left"&gt;
-&lt;div class="liner-continer"&gt;
-&lt;h4 class="woodmart-title-container title wd-fontsize-l"&gt;Features &amp;amp; Compatibility&lt;/h4&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
+          <t>&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
 &lt;div class="elementor-widget-container"&gt;
 &lt;p&gt;Heart-cut lab-diamond studs will leave everyone amazed. Set in 18k gold, Heart Shape diamond of the highest quality was specially selected by our gemologist to create a downfall of amorous sparkle.&lt;/p&gt;
 &lt;ul&gt;
@@ -938,21 +872,7 @@
 &lt;li&gt;Perfect for everyone&lt;/li&gt;
 &lt;/ul&gt;
 &lt;p&gt;This piece is Custom made to order. Expected delivery within 7-10 days. Upon completion, your new heirloom will be dispatched using your chosen shipping method selected at checkout.&lt;/p&gt;
-&lt;p&gt;Have a special date in mind? Reach out to &lt;a class="__cf_email__" data-cfemail="c3b0a2afa6b083a2aeacb1a6b7abaaa0a2eda0acae" href="/cdn-cgi/l/email-protection"&gt;[email protected]&lt;/a&gt; as we may be able to accommodate a rush order for you.&lt;/p&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-c127cd8 elementor-widget elementor-widget-wd_button" data-element_type="widget" data-id="c127cd8" data-widget_type="wd_button.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-button.min.css?ver=8.1.1" id="wd-button-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="wd-button-wrapper text-center wd-collapsible-button"&gt;
-&lt;a class="btn btn-style-link btn-shape- btn-size-default btn-color-primary btn-icon-pos-right" href="#"&gt;
-&lt;span class="wd-btn-text" data-elementor-setting-key="text"&gt;
-					SHOW MORE				&lt;/span&gt;
-&lt;span class="wd-btn-icon"&gt;
-&lt;svg class="wd-icon e-font-icon-svg e-fas-chevron-down" viewbox="0 0 448 512" xmlns="http://www.w3.org/2000/svg"&gt;&lt;path d="M207.029 381.476L12.686 187.132c-9.373-9.373-9.373-24.569 0-33.941l22.667-22.667c9.357-9.357 24.522-9.375 33.901-.04L224 284.505l154.745-154.021c9.379-9.335 24.544-9.317 33.901.04l22.667 22.667c9.373 9.373 9.373 24.569 0 33.941L240.971 381.476c-9.373 9.372-24.569 9.372-33.942 0z"&gt;&lt;/path&gt;&lt;/svg&gt; &lt;/span&gt;
-&lt;/a&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
+&lt;p&gt;Have a special date in mind? Reach out to &lt;a class="__cf_email__" data-cfemail="5625373a332516373b392433223e3f35377835393b" href="/cdn-cgi/l/email-protection"&gt;[email protected]&lt;/a&gt; as we may be able to accommodate a rush order for you.&lt;/p&gt;
 &lt;/div&gt;
 &lt;/div&gt;</t>
         </is>
@@ -1005,7 +925,12 @@
       </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>men</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -1031,18 +956,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>&lt;div class="wd-negative-gap elementor-element elementor-element-aa67a64 wd-section-stretch wd-collapsible-content e-flex e-con-boxed e-con e-parent" data-element_type="container" data-id="aa67a64"&gt;
-&lt;div class="e-con-inner"&gt;
-&lt;div class="elementor-element elementor-element-81ef30d wd-width-100 elementor-widget elementor-widget-wd_title" data-element_type="widget" data-id="81ef30d" data-widget_type="wd_title.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-section-title.min.css?ver=8.1.1" id="wd-section-title-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="title-wrapper wd-set-mb reset-last-child wd-title-color-default wd-title-style-default wd-title-size-default text-left"&gt;
-&lt;div class="liner-continer"&gt;
-&lt;h4 class="woodmart-title-container title wd-fontsize-l"&gt;Features &amp;amp; Compatibility&lt;/h4&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
+          <t>&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
 &lt;div class="elementor-widget-container"&gt;
 &lt;p style="padding: 0px; margin: 0px 0px 1.43rem; line-height: inherit; font-size: 16px; font-family: Nunito, sans-serif; font-style: normal; font-weight: 300; letter-spacing: normal; text-align: start; text-indent: 0px; text-transform: none; text-decoration: none;"&gt;The “Lumière” Radiant Ring, with its pave diamond arrangement, promises eternal brilliance and grace. Elegant, yet modern design will make you sparkle every day ✨&lt;/p&gt;
 &lt;ul style="padding: 0px 0px 0px 20px; margin: 0px 0px 1.43em; font-family: Nunito, sans-serif; font-size: 16px; font-style: normal; font-weight: 300; letter-spacing: normal; text-align: start; text-indent: 0px; text-transform: none; text-decoration: none;"&gt;
@@ -1052,20 +966,6 @@
 &lt;li style="padding: 0px; margin: 0px 0px 0px 5px; line-height: 1.8; font-size: 1.14rem;"&gt;Perfect for every woman&lt;/li&gt;
 &lt;/ul&gt;
 &lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-c127cd8 elementor-widget elementor-widget-wd_button" data-element_type="widget" data-id="c127cd8" data-widget_type="wd_button.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-button.min.css?ver=8.1.1" id="wd-button-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="wd-button-wrapper text-center wd-collapsible-button"&gt;
-&lt;a class="btn btn-style-link btn-shape- btn-size-default btn-color-primary btn-icon-pos-right" href="#"&gt;
-&lt;span class="wd-btn-text" data-elementor-setting-key="text"&gt;
-					SHOW MORE				&lt;/span&gt;
-&lt;span class="wd-btn-icon"&gt;
-&lt;svg class="wd-icon e-font-icon-svg e-fas-chevron-down" viewbox="0 0 448 512" xmlns="http://www.w3.org/2000/svg"&gt;&lt;path d="M207.029 381.476L12.686 187.132c-9.373-9.373-9.373-24.569 0-33.941l22.667-22.667c9.357-9.357 24.522-9.375 33.901-.04L224 284.505l154.745-154.021c9.379-9.335 24.544-9.317 33.901.04l22.667 22.667c9.373 9.373 9.373 24.569 0 33.941L240.971 381.476c-9.373 9.372-24.569 9.372-33.942 0z"&gt;&lt;/path&gt;&lt;/svg&gt; &lt;/span&gt;
-&lt;/a&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
 &lt;/div&gt;</t>
         </is>
       </c>
@@ -1119,6 +1019,11 @@
       <c r="U6" t="n">
         <v>1</v>
       </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>men</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1143,18 +1048,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>&lt;div class="wd-negative-gap elementor-element elementor-element-aa67a64 wd-section-stretch wd-collapsible-content e-flex e-con-boxed e-con e-parent" data-element_type="container" data-id="aa67a64"&gt;
-&lt;div class="e-con-inner"&gt;
-&lt;div class="elementor-element elementor-element-81ef30d wd-width-100 elementor-widget elementor-widget-wd_title" data-element_type="widget" data-id="81ef30d" data-widget_type="wd_title.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-section-title.min.css?ver=8.1.1" id="wd-section-title-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="title-wrapper wd-set-mb reset-last-child wd-title-color-default wd-title-style-default wd-title-size-default text-left"&gt;
-&lt;div class="liner-continer"&gt;
-&lt;h4 class="woodmart-title-container title wd-fontsize-l"&gt;Features &amp;amp; Compatibility&lt;/h4&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
+          <t>&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
 &lt;div class="elementor-widget-container"&gt;
 &lt;p&gt;Luna is a bezel set lab grown diamond ring in yellow 18k gold. Perfect for everyday and evening as a statement piece. You will love its shine and elegance with a touch of modern day.&lt;/p&gt;
 &lt;p&gt;• 1.50 ct Lab grown diamond&lt;/p&gt;
@@ -1165,20 +1059,6 @@
 &lt;p&gt;• Perfect for everyone&lt;/p&gt;
 &lt;p&gt;• For any occasion&lt;/p&gt;
 &lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-c127cd8 elementor-widget elementor-widget-wd_button" data-element_type="widget" data-id="c127cd8" data-widget_type="wd_button.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-button.min.css?ver=8.1.1" id="wd-button-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="wd-button-wrapper text-center wd-collapsible-button"&gt;
-&lt;a class="btn btn-style-link btn-shape- btn-size-default btn-color-primary btn-icon-pos-right" href="#"&gt;
-&lt;span class="wd-btn-text" data-elementor-setting-key="text"&gt;
-					SHOW MORE				&lt;/span&gt;
-&lt;span class="wd-btn-icon"&gt;
-&lt;svg class="wd-icon e-font-icon-svg e-fas-chevron-down" viewbox="0 0 448 512" xmlns="http://www.w3.org/2000/svg"&gt;&lt;path d="M207.029 381.476L12.686 187.132c-9.373-9.373-9.373-24.569 0-33.941l22.667-22.667c9.357-9.357 24.522-9.375 33.901-.04L224 284.505l154.745-154.021c9.379-9.335 24.544-9.317 33.901.04l22.667 22.667c9.373 9.373 9.373 24.569 0 33.941L240.971 381.476c-9.373 9.372-24.569 9.372-33.942 0z"&gt;&lt;/path&gt;&lt;/svg&gt; &lt;/span&gt;
-&lt;/a&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
 &lt;/div&gt;</t>
         </is>
       </c>
@@ -1230,7 +1110,12 @@
       </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="n">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>men</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -1256,18 +1141,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>&lt;div class="wd-negative-gap elementor-element elementor-element-aa67a64 wd-section-stretch wd-collapsible-content e-flex e-con-boxed e-con e-parent" data-element_type="container" data-id="aa67a64"&gt;
-&lt;div class="e-con-inner"&gt;
-&lt;div class="elementor-element elementor-element-81ef30d wd-width-100 elementor-widget elementor-widget-wd_title" data-element_type="widget" data-id="81ef30d" data-widget_type="wd_title.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;div class="title-wrapper wd-set-mb reset-last-child wd-title-color-default wd-title-style-default wd-title-size-default text-left"&gt;
-&lt;div class="liner-continer"&gt;
-&lt;h4 class="woodmart-title-container title wd-fontsize-l"&gt;Features &amp;amp; Compatibility&lt;/h4&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
+          <t>&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
 &lt;div class="elementor-widget-container"&gt;
 &lt;p&gt;Our best-selling engagement ring which you can wear as a stand alone piece everyday or for a night out.&lt;/p&gt;
 &lt;p&gt;– Lab-grown diamond&lt;/p&gt;
@@ -1276,20 +1150,6 @@
 &lt;p&gt;– 18k solid gold&lt;/p&gt;
 &lt;p&gt;– Approx. 2 gm&lt;/p&gt;
 &lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-c127cd8 elementor-widget elementor-widget-wd_button" data-element_type="widget" data-id="c127cd8" data-widget_type="wd_button.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;div class="wd-button-wrapper text-center wd-collapsible-button"&gt;
-&lt;a class="btn btn-style-link btn-shape- btn-size-default btn-color-primary btn-icon-pos-right" href="#"&gt;
-&lt;span class="wd-btn-text" data-elementor-setting-key="text"&gt;
-					SHOW MORE				&lt;/span&gt;
-&lt;span class="wd-btn-icon"&gt;
-&lt;svg class="wd-icon e-font-icon-svg e-fas-chevron-down" viewbox="0 0 448 512" xmlns="http://www.w3.org/2000/svg"&gt;&lt;path d="M207.029 381.476L12.686 187.132c-9.373-9.373-9.373-24.569 0-33.941l22.667-22.667c9.357-9.357 24.522-9.375 33.901-.04L224 284.505l154.745-154.021c9.379-9.335 24.544-9.317 33.901.04l22.667 22.667c9.373 9.373 9.373 24.569 0 33.941L240.971 381.476c-9.373 9.372-24.569 9.372-33.942 0z"&gt;&lt;/path&gt;&lt;/svg&gt; &lt;/span&gt;
-&lt;/a&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
 &lt;/div&gt;</t>
         </is>
       </c>
@@ -1341,7 +1201,12 @@
       </c>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>men</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -1367,18 +1232,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>&lt;div class="wd-negative-gap elementor-element elementor-element-aa67a64 wd-section-stretch wd-collapsible-content e-flex e-con-boxed e-con e-parent" data-element_type="container" data-id="aa67a64"&gt;
-&lt;div class="e-con-inner"&gt;
-&lt;div class="elementor-element elementor-element-81ef30d wd-width-100 elementor-widget elementor-widget-wd_title" data-element_type="widget" data-id="81ef30d" data-widget_type="wd_title.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;div class="title-wrapper wd-set-mb reset-last-child wd-title-color-default wd-title-style-default wd-title-size-default text-left"&gt;
-&lt;div class="liner-continer"&gt;
-&lt;h4 class="woodmart-title-container title wd-fontsize-l"&gt;Features &amp;amp; Compatibility&lt;/h4&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
+          <t>&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
 &lt;div class="elementor-widget-container"&gt;
 &lt;p&gt;&lt;em&gt;Soleil&lt;/em&gt; is a Yellow Cushion diamond ring, featuring 1.5 ct Fancy Yellow lab-grown diamond with 0.15 ct each side stones. It’s for someone bold and ready to express themselves. Set in 18k white gold, Cushion lab diamond ads timeless elegance.&lt;/p&gt;
 &lt;p&gt;• Cushion lab-grown diamond&lt;/p&gt;
@@ -1387,21 +1241,7 @@
 &lt;p&gt;• 18k white gold, Approx. 2.5 gm&lt;/p&gt;
 &lt;p&gt;• Perfect for a special occasion&lt;/p&gt;
 &lt;p&gt;&lt;em&gt;This piece is Custom made to order. Expected delivery within 7-10 days. Upon completion, your new heirloom will be dispatched using your chosen shipping method selected at checkout.&lt;/em&gt;&lt;/p&gt;
-&lt;p&gt;Have a special date in mind? Reach out to&lt;span class="Apple-converted-space"&gt; &lt;/span&gt;&lt;em&gt;&lt;a class="__cf_email__" data-cfemail="4734262b223407262a283522332f2e24266924282a" href="/cdn-cgi/l/email-protection"&gt;[email protected]&lt;/a&gt;&lt;/em&gt;&lt;span class="Apple-converted-space"&gt; &lt;/span&gt;as we may be able to accommodate a rush order for&lt;span class="Apple-converted-space"&gt; &lt;/span&gt;you&lt;span class="Apple-converted-space"&gt; &lt;/span&gt;&lt;span class="Apple-converted-space"&gt;💫&lt;/span&gt;&lt;/p&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-c127cd8 elementor-widget elementor-widget-wd_button" data-element_type="widget" data-id="c127cd8" data-widget_type="wd_button.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;div class="wd-button-wrapper text-center wd-collapsible-button"&gt;
-&lt;a class="btn btn-style-link btn-shape- btn-size-default btn-color-primary btn-icon-pos-right" href="#"&gt;
-&lt;span class="wd-btn-text" data-elementor-setting-key="text"&gt;
-					SHOW MORE				&lt;/span&gt;
-&lt;span class="wd-btn-icon"&gt;
-&lt;svg class="wd-icon e-font-icon-svg e-fas-chevron-down" viewbox="0 0 448 512" xmlns="http://www.w3.org/2000/svg"&gt;&lt;path d="M207.029 381.476L12.686 187.132c-9.373-9.373-9.373-24.569 0-33.941l22.667-22.667c9.357-9.357 24.522-9.375 33.901-.04L224 284.505l154.745-154.021c9.379-9.335 24.544-9.317 33.901.04l22.667 22.667c9.373 9.373 9.373 24.569 0 33.941L240.971 381.476c-9.373 9.372-24.569 9.372-33.942 0z"&gt;&lt;/path&gt;&lt;/svg&gt; &lt;/span&gt;
-&lt;/a&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
+&lt;p&gt;Have a special date in mind? Reach out to&lt;span class="Apple-converted-space"&gt; &lt;/span&gt;&lt;em&gt;&lt;a class="__cf_email__" data-cfemail="285b49444d5b684945475a4d5c40414b49064b4745" href="/cdn-cgi/l/email-protection"&gt;[email protected]&lt;/a&gt;&lt;/em&gt;&lt;span class="Apple-converted-space"&gt; &lt;/span&gt;as we may be able to accommodate a rush order for&lt;span class="Apple-converted-space"&gt; &lt;/span&gt;you&lt;span class="Apple-converted-space"&gt; &lt;/span&gt;&lt;span class="Apple-converted-space"&gt;💫&lt;/span&gt;&lt;/p&gt;
 &lt;/div&gt;
 &lt;/div&gt;</t>
         </is>
@@ -1454,7 +1294,12 @@
       </c>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>men</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -1480,18 +1325,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>&lt;div class="wd-negative-gap elementor-element elementor-element-aa67a64 wd-section-stretch wd-collapsible-content e-flex e-con-boxed e-con e-parent" data-element_type="container" data-id="aa67a64"&gt;
-&lt;div class="e-con-inner"&gt;
-&lt;div class="elementor-element elementor-element-81ef30d wd-width-100 elementor-widget elementor-widget-wd_title" data-element_type="widget" data-id="81ef30d" data-widget_type="wd_title.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-section-title.min.css?ver=8.1.1" id="wd-section-title-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="title-wrapper wd-set-mb reset-last-child wd-title-color-default wd-title-style-default wd-title-size-default text-left"&gt;
-&lt;div class="liner-continer"&gt;
-&lt;h4 class="woodmart-title-container title wd-fontsize-l"&gt;Features &amp;amp; Compatibility&lt;/h4&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
+          <t>&lt;div class="elementor-element elementor-element-832e588 wd-single-content elementor-widget elementor-widget-wd_single_product_content" data-element_type="widget" data-id="832e588" data-widget_type="wd_single_product_content.default"&gt;
 &lt;div class="elementor-widget-container"&gt;
 &lt;p&gt;The Oval Ring, with its classic solitaire arrangement, promises eternal brilliance and grace. Elegant, yet modern design will make you sparkle every day ✨&lt;/p&gt;
 &lt;ul style="padding: 0px 0px 0px 20px;margin: 0px 0px 1.43em;font-family: Nunito, sans-serif;font-style: normal;font-weight: 300;letter-spacing: normal;text-align: start;text-indent: 0px;text-transform: none;text-decoration: none;font-size: 16px"&gt;
@@ -1501,20 +1335,6 @@
 &lt;li style="padding: 0px;margin: 0px 0px 0px 5px;line-height: 1.8;font-size: 1.14rem"&gt;Perfect for every woman&lt;/li&gt;
 &lt;/ul&gt;
 &lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="elementor-element elementor-element-c127cd8 elementor-widget elementor-widget-wd_button" data-element_type="widget" data-id="c127cd8" data-widget_type="wd_button.default"&gt;
-&lt;div class="elementor-widget-container"&gt;
-&lt;link href="https://www.amorethica.com/wp-content/themes/woodmart/css/parts/el-button.min.css?ver=8.1.1" id="wd-button-css" media="all" rel="stylesheet" type="text/css"/&gt; &lt;div class="wd-button-wrapper text-center wd-collapsible-button"&gt;
-&lt;a class="btn btn-style-link btn-shape- btn-size-default btn-color-primary btn-icon-pos-right" href="#"&gt;
-&lt;span class="wd-btn-text" data-elementor-setting-key="text"&gt;
-					SHOW MORE				&lt;/span&gt;
-&lt;span class="wd-btn-icon"&gt;
-&lt;svg class="wd-icon e-font-icon-svg e-fas-chevron-down" viewbox="0 0 448 512" xmlns="http://www.w3.org/2000/svg"&gt;&lt;path d="M207.029 381.476L12.686 187.132c-9.373-9.373-9.373-24.569 0-33.941l22.667-22.667c9.357-9.357 24.522-9.375 33.901-.04L224 284.505l154.745-154.021c9.379-9.335 24.544-9.317 33.901.04l22.667 22.667c9.373 9.373 9.373 24.569 0 33.941L240.971 381.476c-9.373 9.372-24.569 9.372-33.942 0z"&gt;&lt;/path&gt;&lt;/svg&gt; &lt;/span&gt;
-&lt;/a&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;/div&gt;
 &lt;/div&gt;</t>
         </is>
       </c>
@@ -1566,7 +1386,12 @@
       </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>men</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>